<commit_message>
-Finished the notebook on analysing CRT with dichotomous items. Adjusted mode, stats, and item analysis. Removed standard scores and IF flagged questions.
</commit_message>
<xml_diff>
--- a/Data analytics/Language tests/Data/one_test_dichotomous_analysis_CRT.xlsx
+++ b/Data analytics/Language tests/Data/one_test_dichotomous_analysis_CRT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
   <si>
     <t>Student</t>
   </si>
@@ -88,12 +88,6 @@
     <t>Mastery?</t>
   </si>
   <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Student09</t>
   </si>
   <si>
@@ -199,10 +193,10 @@
     <t>Item discrimination</t>
   </si>
   <si>
-    <t>ID(UL)</t>
-  </si>
-  <si>
-    <t>r(p-bis)</t>
+    <t>B-index</t>
+  </si>
+  <si>
+    <t>Ф</t>
   </si>
   <si>
     <t>Flagged</t>
@@ -351,15 +345,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>125689</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>24825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -377,7 +371,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4267200" y="9144000"/>
+          <a:off x="3657600" y="8953500"/>
           <a:ext cx="10488889" cy="4596825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -391,9 +385,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Z31" totalsRowShown="0">
-  <autoFilter ref="A1:Z31"/>
-  <tableColumns count="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:X31" totalsRowShown="0">
+  <autoFilter ref="A1:X31"/>
+  <tableColumns count="24">
     <tableColumn id="1" name="Student"/>
     <tableColumn id="2" name="Q01"/>
     <tableColumn id="3" name="Q02"/>
@@ -418,8 +412,6 @@
     <tableColumn id="22" name="Total"/>
     <tableColumn id="23" name="% Correct"/>
     <tableColumn id="24" name="Mastery?"/>
-    <tableColumn id="25" name="z"/>
-    <tableColumn id="26" name="T"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -710,13 +702,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z69"/>
+  <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -789,16 +781,10 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
         <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26">
-      <c r="A2" t="s">
-        <v>26</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -869,16 +855,10 @@
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="Y2">
-        <v>2.3</v>
-      </c>
-      <c r="Z2">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -949,16 +929,10 @@
       <c r="X3">
         <v>1</v>
       </c>
-      <c r="Y3">
-        <v>1.4</v>
-      </c>
-      <c r="Z3">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1029,16 +1003,10 @@
       <c r="X4">
         <v>1</v>
       </c>
-      <c r="Y4">
-        <v>1.4</v>
-      </c>
-      <c r="Z4">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26">
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1109,16 +1077,10 @@
       <c r="X5">
         <v>1</v>
       </c>
-      <c r="Y5">
-        <v>1.4</v>
-      </c>
-      <c r="Z5">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1189,16 +1151,10 @@
       <c r="X6">
         <v>1</v>
       </c>
-      <c r="Y6">
-        <v>0.9</v>
-      </c>
-      <c r="Z6">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1269,16 +1225,10 @@
       <c r="X7">
         <v>1</v>
       </c>
-      <c r="Y7">
-        <v>0.9</v>
-      </c>
-      <c r="Z7">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1349,16 +1299,10 @@
       <c r="X8">
         <v>1</v>
       </c>
-      <c r="Y8">
-        <v>0.9</v>
-      </c>
-      <c r="Z8">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1429,16 +1373,10 @@
       <c r="X9">
         <v>0</v>
       </c>
-      <c r="Y9">
-        <v>0.6</v>
-      </c>
-      <c r="Z9">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1509,16 +1447,10 @@
       <c r="X10">
         <v>0</v>
       </c>
-      <c r="Y10">
-        <v>0.6</v>
-      </c>
-      <c r="Z10">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1589,16 +1521,10 @@
       <c r="X11">
         <v>0</v>
       </c>
-      <c r="Y11">
-        <v>0.6</v>
-      </c>
-      <c r="Z11">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1669,16 +1595,10 @@
       <c r="X12">
         <v>0</v>
       </c>
-      <c r="Y12">
-        <v>0.3</v>
-      </c>
-      <c r="Z12">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1749,16 +1669,10 @@
       <c r="X13">
         <v>0</v>
       </c>
-      <c r="Y13">
-        <v>0.3</v>
-      </c>
-      <c r="Z13">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26">
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1829,16 +1743,10 @@
       <c r="X14">
         <v>0</v>
       </c>
-      <c r="Y14">
-        <v>0.3</v>
-      </c>
-      <c r="Z14">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1909,16 +1817,10 @@
       <c r="X15">
         <v>0</v>
       </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1989,16 +1891,10 @@
       <c r="X16">
         <v>0</v>
       </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="Z16">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26">
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2069,16 +1965,10 @@
       <c r="X17">
         <v>0</v>
       </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26">
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2149,16 +2039,10 @@
       <c r="X18">
         <v>0</v>
       </c>
-      <c r="Y18">
-        <v>-0.2</v>
-      </c>
-      <c r="Z18">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26">
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2229,16 +2113,10 @@
       <c r="X19">
         <v>0</v>
       </c>
-      <c r="Y19">
-        <v>-0.2</v>
-      </c>
-      <c r="Z19">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26">
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2309,16 +2187,10 @@
       <c r="X20">
         <v>0</v>
       </c>
-      <c r="Y20">
-        <v>-0.2</v>
-      </c>
-      <c r="Z20">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26">
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2389,16 +2261,10 @@
       <c r="X21">
         <v>0</v>
       </c>
-      <c r="Y21">
-        <v>-0.2</v>
-      </c>
-      <c r="Z21">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26">
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2469,16 +2335,10 @@
       <c r="X22">
         <v>0</v>
       </c>
-      <c r="Y22">
-        <v>-0.8</v>
-      </c>
-      <c r="Z22">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26">
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2549,16 +2409,10 @@
       <c r="X23">
         <v>0</v>
       </c>
-      <c r="Y23">
-        <v>-0.8</v>
-      </c>
-      <c r="Z23">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26">
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2629,16 +2483,10 @@
       <c r="X24">
         <v>0</v>
       </c>
-      <c r="Y24">
-        <v>-0.8</v>
-      </c>
-      <c r="Z24">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26">
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2709,16 +2557,10 @@
       <c r="X25">
         <v>0</v>
       </c>
-      <c r="Y25">
-        <v>-0.8</v>
-      </c>
-      <c r="Z25">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26">
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2789,16 +2631,10 @@
       <c r="X26">
         <v>0</v>
       </c>
-      <c r="Y26">
-        <v>-1.1</v>
-      </c>
-      <c r="Z26">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26">
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2869,16 +2705,10 @@
       <c r="X27">
         <v>0</v>
       </c>
-      <c r="Y27">
-        <v>-1.1</v>
-      </c>
-      <c r="Z27">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26">
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2949,16 +2779,10 @@
       <c r="X28">
         <v>0</v>
       </c>
-      <c r="Y28">
-        <v>-1.1</v>
-      </c>
-      <c r="Z28">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26">
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3029,16 +2853,10 @@
       <c r="X29">
         <v>0</v>
       </c>
-      <c r="Y29">
-        <v>-1.1</v>
-      </c>
-      <c r="Z29">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26">
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -3109,16 +2927,10 @@
       <c r="X30">
         <v>0</v>
       </c>
-      <c r="Y30">
-        <v>-1.6</v>
-      </c>
-      <c r="Z30">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26">
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -3189,16 +3001,10 @@
       <c r="X31">
         <v>0</v>
       </c>
-      <c r="Y31">
-        <v>-2.2</v>
-      </c>
-      <c r="Z31">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>1</v>
@@ -3260,13 +3066,10 @@
       <c r="U34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V34" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B35">
         <v>0.533</v>
@@ -3328,149 +3131,140 @@
       <c r="U35">
         <v>0.5</v>
       </c>
-      <c r="V35">
-        <v>0.233</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36">
+        <v>0.857</v>
+      </c>
+      <c r="C36">
+        <v>0.857</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0.857</v>
+      </c>
+      <c r="H36">
+        <v>0.571</v>
+      </c>
+      <c r="I36">
+        <v>0.714</v>
+      </c>
+      <c r="J36">
+        <v>0.857</v>
+      </c>
+      <c r="K36">
+        <v>0.429</v>
+      </c>
+      <c r="L36">
+        <v>0.857</v>
+      </c>
+      <c r="M36">
+        <v>0.714</v>
+      </c>
+      <c r="N36">
+        <v>0.857</v>
+      </c>
+      <c r="O36">
+        <v>0.857</v>
+      </c>
+      <c r="P36">
+        <v>0.714</v>
+      </c>
+      <c r="Q36">
+        <v>0.429</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>0.714</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>0.286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37">
+        <v>0.435</v>
+      </c>
+      <c r="C37">
+        <v>0.435</v>
+      </c>
+      <c r="D37">
+        <v>0.261</v>
+      </c>
+      <c r="E37">
+        <v>0.522</v>
+      </c>
+      <c r="F37">
+        <v>0.348</v>
+      </c>
+      <c r="G37">
+        <v>0.478</v>
+      </c>
+      <c r="H37">
+        <v>0.391</v>
+      </c>
+      <c r="I37">
+        <v>0.304</v>
+      </c>
+      <c r="J37">
+        <v>0.391</v>
+      </c>
+      <c r="K37">
+        <v>0.696</v>
+      </c>
+      <c r="L37">
+        <v>0.478</v>
+      </c>
+      <c r="M37">
+        <v>0.609</v>
+      </c>
+      <c r="N37">
+        <v>0.652</v>
+      </c>
+      <c r="O37">
+        <v>0.174</v>
+      </c>
+      <c r="P37">
+        <v>0.609</v>
+      </c>
+      <c r="Q37">
+        <v>0.13</v>
+      </c>
+      <c r="R37">
+        <v>0.652</v>
+      </c>
+      <c r="S37">
+        <v>0.522</v>
+      </c>
+      <c r="T37">
+        <v>0.739</v>
+      </c>
+      <c r="U37">
+        <v>0.5649999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B36">
-        <v>0.8</v>
-      </c>
-      <c r="C36">
-        <v>0.8</v>
-      </c>
-      <c r="D36">
-        <v>0.9</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>0.7</v>
-      </c>
-      <c r="H36">
-        <v>0.5</v>
-      </c>
-      <c r="I36">
-        <v>0.7</v>
-      </c>
-      <c r="J36">
-        <v>0.9</v>
-      </c>
-      <c r="K36">
-        <v>0.5</v>
-      </c>
-      <c r="L36">
-        <v>0.8</v>
-      </c>
-      <c r="M36">
-        <v>0.7</v>
-      </c>
-      <c r="N36">
-        <v>0.9</v>
-      </c>
-      <c r="O36">
-        <v>0.7</v>
-      </c>
-      <c r="P36">
-        <v>0.8</v>
-      </c>
-      <c r="Q36">
-        <v>0.4</v>
-      </c>
-      <c r="R36">
-        <v>1</v>
-      </c>
-      <c r="S36">
-        <v>0.6</v>
-      </c>
-      <c r="T36">
-        <v>0.9</v>
-      </c>
-      <c r="U36">
-        <v>0.2</v>
-      </c>
-      <c r="V36">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
-      <c r="A37" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37">
-        <v>0.1</v>
-      </c>
-      <c r="C37">
-        <v>0.2</v>
-      </c>
-      <c r="D37">
-        <v>0.3</v>
-      </c>
-      <c r="E37">
-        <v>0.1</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0.6</v>
-      </c>
-      <c r="H37">
-        <v>0.1</v>
-      </c>
-      <c r="I37">
-        <v>0.3</v>
-      </c>
-      <c r="J37">
-        <v>0.1</v>
-      </c>
-      <c r="K37">
-        <v>0.9</v>
-      </c>
-      <c r="L37">
-        <v>0.4</v>
-      </c>
-      <c r="M37">
-        <v>0.5</v>
-      </c>
-      <c r="N37">
-        <v>0.4</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <v>0.3</v>
-      </c>
-      <c r="Q37">
-        <v>0.1</v>
-      </c>
-      <c r="R37">
-        <v>0.3</v>
-      </c>
-      <c r="S37">
-        <v>0.7</v>
-      </c>
-      <c r="T37">
-        <v>0.7</v>
-      </c>
-      <c r="U37">
-        <v>0.7</v>
-      </c>
-      <c r="V37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22">
-      <c r="A39" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>1</v>
@@ -3532,149 +3326,140 @@
       <c r="U39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V39" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22">
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40">
+        <v>0.422</v>
+      </c>
+      <c r="C40">
+        <v>0.422</v>
+      </c>
+      <c r="D40">
+        <v>0.739</v>
+      </c>
+      <c r="E40">
+        <v>0.478</v>
+      </c>
+      <c r="F40">
+        <v>0.652</v>
+      </c>
+      <c r="G40">
+        <v>0.379</v>
+      </c>
+      <c r="H40">
+        <v>0.1799999999999999</v>
+      </c>
+      <c r="I40">
+        <v>0.41</v>
+      </c>
+      <c r="J40">
+        <v>0.466</v>
+      </c>
+      <c r="K40">
+        <v>-0.267</v>
+      </c>
+      <c r="L40">
+        <v>0.379</v>
+      </c>
+      <c r="M40">
+        <v>0.105</v>
+      </c>
+      <c r="N40">
+        <v>0.205</v>
+      </c>
+      <c r="O40">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="P40">
+        <v>0.105</v>
+      </c>
+      <c r="Q40">
+        <v>0.299</v>
+      </c>
+      <c r="R40">
+        <v>0.348</v>
+      </c>
+      <c r="S40">
+        <v>0.1919999999999999</v>
+      </c>
+      <c r="T40">
+        <v>0.261</v>
+      </c>
+      <c r="U40">
+        <v>-0.279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41">
+        <v>0.358</v>
+      </c>
+      <c r="C41">
+        <v>0.358</v>
+      </c>
+      <c r="D41">
+        <v>0.631</v>
+      </c>
+      <c r="E41">
+        <v>0.42</v>
+      </c>
+      <c r="F41">
+        <v>0.552</v>
+      </c>
+      <c r="G41">
+        <v>0.323</v>
+      </c>
+      <c r="H41">
+        <v>0.154</v>
+      </c>
+      <c r="I41">
+        <v>0.354</v>
+      </c>
+      <c r="J41">
+        <v>0.394</v>
+      </c>
+      <c r="K41">
+        <v>-0.234</v>
+      </c>
+      <c r="L41">
+        <v>0.323</v>
+      </c>
+      <c r="M41">
+        <v>0.093</v>
+      </c>
+      <c r="N41">
+        <v>0.189</v>
+      </c>
+      <c r="O41">
+        <v>0.613</v>
+      </c>
+      <c r="P41">
+        <v>0.093</v>
+      </c>
+      <c r="Q41">
+        <v>0.315</v>
+      </c>
+      <c r="R41">
+        <v>0.333</v>
+      </c>
+      <c r="S41">
+        <v>0.164</v>
+      </c>
+      <c r="T41">
+        <v>0.276</v>
+      </c>
+      <c r="U41">
+        <v>-0.236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B40">
-        <v>0.7000000000000001</v>
-      </c>
-      <c r="C40">
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="D40">
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="E40">
-        <v>0.9</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40">
-        <v>0.09999999999999998</v>
-      </c>
-      <c r="H40">
-        <v>0.4</v>
-      </c>
-      <c r="I40">
-        <v>0.4</v>
-      </c>
-      <c r="J40">
-        <v>0.8</v>
-      </c>
-      <c r="K40">
-        <v>-0.4</v>
-      </c>
-      <c r="L40">
-        <v>0.4</v>
-      </c>
-      <c r="M40">
-        <v>0.2</v>
-      </c>
-      <c r="N40">
-        <v>0.5</v>
-      </c>
-      <c r="O40">
-        <v>0.7</v>
-      </c>
-      <c r="P40">
-        <v>0.5</v>
-      </c>
-      <c r="Q40">
-        <v>0.3</v>
-      </c>
-      <c r="R40">
-        <v>0.7</v>
-      </c>
-      <c r="S40">
-        <v>-0.09999999999999998</v>
-      </c>
-      <c r="T40">
-        <v>0.2000000000000001</v>
-      </c>
-      <c r="U40">
-        <v>-0.4999999999999999</v>
-      </c>
-      <c r="V40">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22">
-      <c r="A41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41">
-        <v>0.61</v>
-      </c>
-      <c r="C41">
-        <v>0.498</v>
-      </c>
-      <c r="D41">
-        <v>0.529</v>
-      </c>
-      <c r="E41">
-        <v>0.699</v>
-      </c>
-      <c r="F41">
-        <v>0.717</v>
-      </c>
-      <c r="G41">
-        <v>0.185</v>
-      </c>
-      <c r="H41">
-        <v>0.398</v>
-      </c>
-      <c r="I41">
-        <v>0.399</v>
-      </c>
-      <c r="J41">
-        <v>0.624</v>
-      </c>
-      <c r="K41">
-        <v>-0.287</v>
-      </c>
-      <c r="L41">
-        <v>0.429</v>
-      </c>
-      <c r="M41">
-        <v>0.158</v>
-      </c>
-      <c r="N41">
-        <v>0.457</v>
-      </c>
-      <c r="O41">
-        <v>0.645</v>
-      </c>
-      <c r="P41">
-        <v>0.506</v>
-      </c>
-      <c r="Q41">
-        <v>0.396</v>
-      </c>
-      <c r="R41">
-        <v>0.6879999999999999</v>
-      </c>
-      <c r="S41">
-        <v>-0.06</v>
-      </c>
-      <c r="T41">
-        <v>0.256</v>
-      </c>
-      <c r="U41">
-        <v>-0.345</v>
-      </c>
-      <c r="V41">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22">
-      <c r="A43" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -3697,30 +3482,69 @@
       <c r="H43" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:22">
+      <c r="I43" s="1">
+        <v>7</v>
+      </c>
+      <c r="J43" s="1">
+        <v>8</v>
+      </c>
+      <c r="K43" s="1">
+        <v>9</v>
+      </c>
+      <c r="L43" s="1">
+        <v>10</v>
+      </c>
+      <c r="M43" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
         <v>16</v>
       </c>
-      <c r="C44" t="s">
+      <c r="J44" t="s">
         <v>17</v>
       </c>
-      <c r="D44" t="s">
+      <c r="K44" t="s">
+        <v>18</v>
+      </c>
+      <c r="L44" t="s">
         <v>19</v>
       </c>
-      <c r="E44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
+      <c r="M44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
@@ -3729,287 +3553,249 @@
         <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F45" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" t="s">
         <v>18</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>19</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
-      <c r="A46" s="1" t="s">
+    <row r="48" spans="1:21">
+      <c r="A48" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="B48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49">
+        <v>10.83333333333333</v>
+      </c>
+      <c r="C49">
+        <v>54.16666666666666</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>55.00000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53">
+        <v>13</v>
+      </c>
+      <c r="C53">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54">
         <v>19</v>
       </c>
-      <c r="G46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50">
-        <v>10.83333333333333</v>
-      </c>
-      <c r="C50">
-        <v>54.16666666666666</v>
-      </c>
-      <c r="D50">
-        <v>-0.01</v>
-      </c>
-      <c r="E50">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B51" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B52">
-        <v>8</v>
-      </c>
-      <c r="C52">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53">
-        <v>11</v>
-      </c>
-      <c r="C53">
-        <v>55.00000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="1" t="s">
+      <c r="C54">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B54">
-        <v>13</v>
-      </c>
-      <c r="C54">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="1" t="s">
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="C55">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B55">
-        <v>19</v>
-      </c>
-      <c r="C55">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="1" t="s">
+      <c r="B56">
+        <v>17</v>
+      </c>
+      <c r="C56">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B56">
-        <v>3</v>
-      </c>
-      <c r="C56">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="1" t="s">
+      <c r="B57">
+        <v>3.578485092263982</v>
+      </c>
+      <c r="C57">
+        <v>17.89242546131991</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B57">
-        <v>17</v>
-      </c>
-      <c r="C57">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="1" t="s">
+      <c r="B58">
+        <v>3.639660208973031</v>
+      </c>
+      <c r="C58">
+        <v>18.19830104486516</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B58">
-        <v>3.578485092263982</v>
-      </c>
-      <c r="C58">
-        <v>17.89242546131991</v>
-      </c>
-      <c r="D58">
-        <v>0.998</v>
-      </c>
-      <c r="E58">
-        <v>9.984</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="1" t="s">
+      <c r="B59">
+        <v>12.80555555555556</v>
+      </c>
+      <c r="C59">
+        <v>3.20138888888889</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B59">
-        <v>3.639660208973031</v>
-      </c>
-      <c r="C59">
-        <v>18.19830104486516</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="1" t="s">
+      <c r="B60">
+        <v>13.24712643678161</v>
+      </c>
+      <c r="C60">
+        <v>3.311781609195403</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B60">
-        <v>12.80555555555556</v>
-      </c>
-      <c r="C60">
-        <v>3.20138888888889</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="1" t="s">
+      <c r="B61">
+        <v>2.5</v>
+      </c>
+      <c r="C61">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B61">
-        <v>13.24712643678161</v>
-      </c>
-      <c r="C61">
-        <v>3.311781609195403</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="1" t="s">
+      <c r="B62">
+        <v>30</v>
+      </c>
+      <c r="C62">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B62">
-        <v>2.5</v>
-      </c>
-      <c r="C62">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="1" t="s">
+      <c r="B63">
+        <v>0.06990099391759312</v>
+      </c>
+      <c r="C63">
+        <v>0.06990099391759404</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B63">
-        <v>30</v>
-      </c>
-      <c r="C63">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="B64">
-        <v>0.06990099391759312</v>
+        <v>0.4268923959512381</v>
       </c>
       <c r="C64">
-        <v>0.06990099391759404</v>
+        <v>0.4268923959512381</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B65">
-        <v>0.4268923959512381</v>
+        <v>0.1637438253305818</v>
       </c>
       <c r="C65">
-        <v>0.4268923959512381</v>
+        <v>0.163743825330584</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66">
-        <v>0.1637438253305818</v>
+        <v>-0.1934961721429884</v>
       </c>
       <c r="C66">
-        <v>0.163743825330584</v>
+        <v>-0.1934961721429884</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B67">
-        <v>-0.1934961721429884</v>
+        <v>0.8327456183576328</v>
       </c>
       <c r="C67">
-        <v>-0.1934961721429884</v>
+        <v>0.8327456183576328</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B68">
-        <v>0.8327456183576328</v>
+        <v>-0.2323592798057679</v>
       </c>
       <c r="C68">
-        <v>0.8327456183576328</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B69">
-        <v>-0.2323592798057679</v>
-      </c>
-      <c r="C69">
         <v>-0.2323592798057679</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-Finished dependability analysis for CRT.
</commit_message>
<xml_diff>
--- a/Data analytics/Language tests/Data/one_test_dichotomous_analysis_CRT.xlsx
+++ b/Data analytics/Language tests/Data/one_test_dichotomous_analysis_CRT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="92">
   <si>
     <t>Student</t>
   </si>
@@ -269,6 +269,27 @@
   </si>
   <si>
     <t>[35.0, 40.0, 50.0]</t>
+  </si>
+  <si>
+    <t>Dependability</t>
+  </si>
+  <si>
+    <t>CIcrt</t>
+  </si>
+  <si>
+    <t>Ф(λ)</t>
+  </si>
+  <si>
+    <t>Reliable?</t>
+  </si>
+  <si>
+    <t>Classification consistency?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -345,13 +366,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>125689</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>24825</xdr:rowOff>
@@ -371,7 +392,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3657600" y="8953500"/>
+          <a:off x="5486400" y="8953500"/>
           <a:ext cx="10488889" cy="4596825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3578,8 +3599,14 @@
       <c r="C48" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="E48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
@@ -3589,8 +3616,14 @@
       <c r="C49">
         <v>54.16666666666666</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="E49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49">
+        <v>0.6881123652196379</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
@@ -3600,8 +3633,14 @@
       <c r="C50" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="E50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
         <v>65</v>
       </c>
@@ -3611,8 +3650,14 @@
       <c r="C51">
         <v>40</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="E51" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F51">
+        <v>0.8110000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
         <v>66</v>
       </c>
@@ -3622,8 +3667,14 @@
       <c r="C52">
         <v>55.00000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="E52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="1" t="s">
         <v>67</v>
       </c>
@@ -3633,8 +3684,14 @@
       <c r="C53">
         <v>65</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="E53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
         <v>68</v>
       </c>
@@ -3645,7 +3702,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
         <v>69</v>
       </c>
@@ -3656,7 +3713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
         <v>70</v>
       </c>
@@ -3667,7 +3724,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
@@ -3678,7 +3735,7 @@
         <v>17.89242546131991</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:6">
       <c r="A58" s="1" t="s">
         <v>72</v>
       </c>
@@ -3689,7 +3746,7 @@
         <v>18.19830104486516</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:6">
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
@@ -3700,7 +3757,7 @@
         <v>3.20138888888889</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:6">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
@@ -3711,7 +3768,7 @@
         <v>3.311781609195403</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:6">
       <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
@@ -3722,7 +3779,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:6">
       <c r="A62" s="1" t="s">
         <v>76</v>
       </c>
@@ -3733,7 +3790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:6">
       <c r="A63" s="1" t="s">
         <v>77</v>
       </c>
@@ -3744,7 +3801,7 @@
         <v>0.06990099391759404</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:6">
       <c r="A64" s="1" t="s">
         <v>78</v>
       </c>

</xml_diff>